<commit_message>
[datetime]: updated test cases for datetime fields
</commit_message>
<xml_diff>
--- a/src/test/resources/sample-files/xlsx_sample_single_sheet.xlsx
+++ b/src/test/resources/sample-files/xlsx_sample_single_sheet.xlsx
@@ -5,92 +5,125 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="169" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Height (mts)</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
-    <t>410, Madison, Seattle, WA – 123456</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>Robin</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>Mountain View, CA</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>Guiliano Carlini</t>
-  </si>
-  <si>
-    <t>Palo Alto, CA – 43234</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>Natasha</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height (mts)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Login Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Session Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-12-1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410, Madison, Seattle, WA – 123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23-12-2023 18:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-06-1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEMALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mountain View, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-11-2023 00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guiliano Carlini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-08-1978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palo Alto, CA – 43234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06-11-2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natasha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-02-1990</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -118,6 +151,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,7 +200,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,37 +209,48 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.75"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8163265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.09"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,104 +272,137 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>32</v>
+        <v>9</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1.8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.104166666666667</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2.1</v>
       </c>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1.68</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0.0245717592592593</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1.78</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>1.85416666666667</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>35</v>
+        <v>29</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0.524305555555556</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>